<commit_message>
Versión funcional con fragmentación semántica
</commit_message>
<xml_diff>
--- a/Datos/indice.xlsx
+++ b/Datos/indice.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\G9-IA\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juandn\Documents\Curso IA g9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFB03A3-60AB-493A-86E8-1A4F12D105E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{988E960D-89FA-4CB1-8671-18C4A779E4FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Identificador</t>
   </si>
@@ -57,13 +56,97 @@
   </si>
   <si>
     <t>Fecha de fin de vigencia</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>Calendario laboral</t>
+  </si>
+  <si>
+    <t>https://intranet.uniovi.es/documents/3676224/10209682/CALENDARIO+LABORAL+2025_PTGAS-PDI_Cons.Gob.+20-12-2024-web.pdf/793fe75c-0f95-7c60-6e46-31143f9d8d42?t=1738919403845</t>
+  </si>
+  <si>
+    <t>CALENDARIO LABORAL 2025_PTGAS-PDI_Cons.Gob. 20-12-2024-web.pdf</t>
+  </si>
+  <si>
+    <t>Vigente</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>convenio colectivo ptgas.pdf</t>
+  </si>
+  <si>
+    <t>Convenio Colectivo PTGAS</t>
+  </si>
+  <si>
+    <t>https://sede.asturias.es/bopa/2013/02/13/2013-02521.pdf</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>Estructura básica de gobierno de la Universidad de Oviedo.pdf</t>
+  </si>
+  <si>
+    <t>https://secretaria.uniovi.es/c/document_library/get_file?uuid=9eb99322-0466-45f1-b978-6ca7a688e82d&amp;groupId=952290</t>
+  </si>
+  <si>
+    <t>2025-04</t>
+  </si>
+  <si>
+    <t>Estructura general de gobierno Uniovi</t>
+  </si>
+  <si>
+    <t>https://secretaria.uniovi.es/c/document_library/get_file?uuid=1f8e6a98-9937-492c-b6c8-27438769a97e&amp;groupId=952290</t>
+  </si>
+  <si>
+    <t>Estructura general de gobierno, funciones y organización administrativa.pdf</t>
+  </si>
+  <si>
+    <t>Estructura básica de gobierno de la Universidad de Oviedo</t>
+  </si>
+  <si>
+    <t>2025-05</t>
+  </si>
+  <si>
+    <t>Reglamento regulador del teletrabajo</t>
+  </si>
+  <si>
+    <t>Reglamento que regula el Teletrabajo como modalidad de presentación de servicios a distancia.pdf</t>
+  </si>
+  <si>
+    <t>https://secretaria.uniovi.es/c/document_library/get_file?uuid=9855f52c-0d08-4cc7-bbde-b8458e2c483b&amp;groupId=952290</t>
+  </si>
+  <si>
+    <t>2025-06</t>
+  </si>
+  <si>
+    <t>Presupuesto Universidad de Oviedo - Contenido General</t>
+  </si>
+  <si>
+    <t>presupuestos Uniovi 2025.pdf</t>
+  </si>
+  <si>
+    <t>https://sede.asturias.es/bopa/2024/12/30/2024-11360.pdf</t>
+  </si>
+  <si>
+    <t>Area de información</t>
+  </si>
+  <si>
+    <t>PTGAS</t>
+  </si>
+  <si>
+    <t>UNIOVI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +167,13 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -107,12 +197,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -448,24 +542,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42A3CF1-6928-4532-B57E-9A5D5E143629}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.125" customWidth="1"/>
+    <col min="4" max="4" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -486,6 +581,165 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45646</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3">
+        <v>41318</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45434</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45461</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3">
+        <v>45659</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3">
+        <v>45657</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3">
+        <v>55153</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>